<commit_message>
as requested by @agruss2 - fixes #134
</commit_message>
<xml_diff>
--- a/src/main/resources/com/github/jhpoelen/fbob/osmose_config/README.xlsx
+++ b/src/main/resources/com/github/jhpoelen/fbob/osmose_config/README.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="23715" windowHeight="9015"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="23715" windowHeight="9015" firstSheet="12" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="osm_all-parameters.csv" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="340">
   <si>
     <t>Parameter</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>osmose.configuration.movement</t>
-  </si>
-  <si>
-    <t>Name of the .csv file providing information about the distribution maps fed into OSMOSE</t>
   </si>
   <si>
     <t>osmose.configuration.mortality.fishing</t>
@@ -801,12 +798,6 @@
     <t>Boolean parameter indicating whether the predation pressures exerted on the different size classes of focal functional groups should be saved in a .csv file or not</t>
   </si>
   <si>
-    <t>Boolean parameter indicating whether spatial estimates of biomasses for focal functional groups should be saved in a .csv file or not</t>
-  </si>
-  <si>
-    <t>Boolean parameter indicating whether spatial estimates of biomasses for background functional groups should be saved in a .csv file or not</t>
-  </si>
-  <si>
     <t>output.step0.include</t>
   </si>
   <si>
@@ -840,9 +831,6 @@
     <t>Maximum size (in cm) of the individuals of all focal functional groups for which OSMOSE computes outputs</t>
   </si>
   <si>
-    <t>Size (in cm) of the size classes of focal functional groups for which OSMOSE computes outputs</t>
-  </si>
-  <si>
     <t>The default value of this parameter is: 10 cm</t>
   </si>
   <si>
@@ -922,9 +910,6 @@
   </si>
   <si>
     <t>Critical predation efficiency of focal functional group X</t>
-  </si>
-  <si>
-    <t>Maximum annual ingestion rate (in years) of focal functional group X</t>
   </si>
   <si>
     <t>Minimum predator/prey size ratio of the juveniles and adults of focal functional group X</t>
@@ -1009,9 +994,6 @@
     <t># The "reproduction-seasonality-spX.csv" file was generated by the bridge between FishBase/SeaLifeBase and OSMOSE</t>
   </si>
   <si>
-    <t># This file provides reproduction seasonality estimates for focal functional group X</t>
-  </si>
-  <si>
     <t>species.name.spX</t>
   </si>
   <si>
@@ -1142,10 +1124,130 @@
     <t>Longevity (in years) of focal functional group X</t>
   </si>
   <si>
-    <t>Please note that this parameter appears after species.maturity.size.spX in the "osm_param-species.csv" file; this entails that the OSMOSE model will consider species.maturity.size.spX rather than species.maturity.age.spX to simulate sexual maturity for focal functional group X. If the user prefers OSMOSE to consider the parameter species.maturity.age.spX to simulate sexual maturity for focal functional group X, then the parameter species.maturity.size.spX should be removed from the "osm_param-species.csv" file</t>
-  </si>
-  <si>
     <t>The user should enter a value for this parameter. The default value provided is: 0.0 cm. Please note that this parameter appears after mortality.fishing.recruitment.age.spX in the "osm_param-fishing.csv" file; this entails that the OSMOSE model will consider mortality.fishing.recruitment.age.spX rather than mortality.fishing.recruitment.size.spX to simulate recruitment into the fisheries for focal functional group X. If the user prefers OSMOSE to consider the parameter mortality.fishing.recruitment.size.spX to simulate the recruitment of focal functional group X into the fisheries, then the parameter mortality.fishing.recruitment.age.spX should be removed from the "osm_param-fishing.csv" file</t>
+  </si>
+  <si>
+    <t>Name of the .csv file providing information about the distribution maps fed into OSMOSE, as well as information on fish and invertebrate movement patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The default value of this parameter is: 0.00053669 g </t>
+  </si>
+  <si>
+    <t>The default value of this parameter is: 0.1 cm</t>
+  </si>
+  <si>
+    <t>The name of focal functional groups should not include spaces nor underscores. For example, "SmallPelagics" is a valid functional group name, but not "Small pelagics" nor "Small_pelagics"</t>
+  </si>
+  <si>
+    <t>A NA ("not available") is provided by the bridge between FishBase/SeaLifeBase and OSMOSE if it was unable to assign a value to this parameter from the information compiled in FishBase and SeaLifeBase</t>
+  </si>
+  <si>
+    <t>A NA ("not available") is provided by the bridge between FishBase/SeaLifeBase and OSMOSE if it was unable to assign a value to this parameter from the information compiled in FishBase and SeaLifeBase. Please note that this parameter appears after species.maturity.size.spX in the "osm_param-species.csv" file; this entails that the OSMOSE model will consider species.maturity.size.spX rather than species.maturity.age.spX to simulate sexual maturity for focal functional group X. If the user prefers OSMOSE to consider the parameter species.maturity.age.spX to simulate sexual maturity for focal functional group X, then the parameter species.maturity.size.spX should be removed from the "osm_param-species.csv" file</t>
+  </si>
+  <si>
+    <t>The default value of this parameter is: 0.5</t>
+  </si>
+  <si>
+    <t>The default value of this parameter is: 1 year</t>
+  </si>
+  <si>
+    <t>The name of background functional groups should not include spaces nor underscores. For example, "InfaunalMeiobenthos" is a valid functional group name, but not "Infaunal meiobenthos" nor "Infaunal_meiobenthos"</t>
+  </si>
+  <si>
+    <r>
+      <t>The default value of this parameter is: 0.2 year</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <t>A default value of 0.0 year is provided by the bridge between FishBase/SeaLifeBase and OSMOSE if it was unable to assign a value to this parameter from the information compiled in FishBase and SeaLifeBase</t>
+  </si>
+  <si>
+    <t>The default value of this parameter is: 0.57</t>
+  </si>
+  <si>
+    <r>
+      <t>Maximum annual ingestion rate (in year</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) of focal functional group X</t>
+    </r>
+  </si>
+  <si>
+    <t>The default value of this parameter is: 3.5 year-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The default value of this parameter is: 3.5 </t>
+  </si>
+  <si>
+    <t>The default value of this parameter is: 30</t>
+  </si>
+  <si>
+    <t>This parameter is actually the body size at sexual maturity of focal functional group X. A default value of 0.0 cm is provided by the bridge between FishBase/SeaLifeBase and OSMOSE if it was unable to assign a value to this parameter from the information compiled in FishBase and SeaLifeBase</t>
+  </si>
+  <si>
+    <t># This file provides reproduction seasonality estimates for focal functional groups</t>
+  </si>
+  <si>
+    <t>Boolean parameter indicating whether spatial estimates of biomasses for focal functional groups should be saved in a .nc file or not</t>
+  </si>
+  <si>
+    <t>Boolean parameter indicating whether spatial estimates of biomasses for background functional groups should be saved in a .nc file or not</t>
+  </si>
+  <si>
+    <t>Range (in cm) of the size classes of focal functional groups for which OSMOSE computes outputs</t>
+  </si>
+  <si>
+    <t>output.distrib.byAge.min</t>
+  </si>
+  <si>
+    <t>output.distrib.byAge.max</t>
+  </si>
+  <si>
+    <t>output.distrib.byAge.incr</t>
+  </si>
+  <si>
+    <t>The default value of this parameter is: 0 year</t>
+  </si>
+  <si>
+    <t>The default value of this parameter is: 10 years</t>
+  </si>
+  <si>
+    <t>Minimum age (in years) of the individuals of all focal functional groups for which OSMOSE computes outputs</t>
+  </si>
+  <si>
+    <t>Maximum age (in years) of the individuals of all focal functional groups for which OSMOSE computes outputs</t>
+  </si>
+  <si>
+    <t>Range (in years) of the age classes of focal functional groups for which OSMOSE computes outputs</t>
   </si>
 </sst>
 </file>
@@ -1997,8 +2099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2048,7 +2150,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2056,7 +2158,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
@@ -2076,7 +2178,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2084,13 +2186,13 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2104,7 +2206,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2118,7 +2220,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2146,7 +2248,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2182,13 +2284,13 @@
         <v>29</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2205,12 +2307,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>33</v>
+        <v>311</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>6</v>
@@ -2221,10 +2323,10 @@
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>6</v>
@@ -2235,10 +2337,10 @@
     </row>
     <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>6</v>
@@ -2249,10 +2351,10 @@
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>6</v>
@@ -2263,10 +2365,10 @@
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>6</v>
@@ -2277,10 +2379,10 @@
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>6</v>
@@ -2291,10 +2393,10 @@
     </row>
     <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>6</v>
@@ -2305,10 +2407,10 @@
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>6</v>
@@ -2319,10 +2421,10 @@
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>6</v>
@@ -2333,10 +2435,10 @@
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>6</v>
@@ -2356,7 +2458,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2383,62 +2485,63 @@
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2447,7 +2550,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2474,128 +2577,128 @@
     </row>
     <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>274</v>
+        <v>323</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>7</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>7</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>7</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -2608,7 +2711,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2635,10 +2738,10 @@
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -2657,7 +2760,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2685,16 +2788,16 @@
     </row>
     <row r="2" spans="1:4" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -2707,19 +2810,19 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -2739,12 +2842,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>287</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -2762,12 +2865,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2780,24 +2883,24 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2807,10 +2910,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2838,86 +2941,86 @@
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2925,13 +3028,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2939,559 +3042,601 @@
         <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>180</v>
-      </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>233</v>
+        <v>329</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>234</v>
+        <v>330</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>246</v>
+        <v>331</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>239</v>
+        <v>332</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>248</v>
+        <v>337</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>174</v>
+        <v>335</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -3503,7 +3648,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3527,138 +3674,138 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="32.25" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>6</v>
@@ -3667,60 +3814,60 @@
         <v>316</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="32.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>7</v>
+        <v>315</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>7</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -3733,7 +3880,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3759,88 +3906,88 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -3853,7 +4000,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3881,114 +4028,114 @@
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -4008,12 +4155,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -4026,19 +4173,19 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -4051,7 +4198,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4079,52 +4226,52 @@
     </row>
     <row r="2" spans="1:4" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
@@ -4144,7 +4291,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4172,16 +4319,16 @@
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -4194,7 +4341,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4208,17 +4355,17 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -4237,100 +4384,100 @@
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>116</v>
-      </c>
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new readme.xlsx as provided by Arnaud related to #144 .
</commit_message>
<xml_diff>
--- a/src/main/resources/com/github/jhpoelen/fbob/osmose_config/README.xlsx
+++ b/src/main/resources/com/github/jhpoelen/fbob/osmose_config/README.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARNAUD\Dropbox\Postdoc_Miami\Postdoc_Miami_November_2017\RESTORE_Act_project\Component 4_RESTORE Act project_6\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="23715" windowHeight="9015" firstSheet="12" activeTab="17"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="23712" windowHeight="9012" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="osm_all-parameters.csv" sheetId="2" r:id="rId1"/>
@@ -219,41 +224,12 @@
     <t># The "osm_ltlbiomass.nc" file provided by the bridge between FishBase/SeaLifeBase and OSMOSE is a template file that was generated for the OSMOSE model of the West Florida Shelf</t>
   </si>
   <si>
-    <t>Name of .csv file providing basic parameter estimates (e.g., parameters of the von Berlafanffy growth relationship) for focal functional groups</t>
-  </si>
-  <si>
     <t>mortality.fishing.rate.spX</t>
   </si>
   <si>
     <t>mortality.fishing.recruitment.age.spX</t>
   </si>
   <si>
-    <r>
-      <t>Annual fishing mortality rate (in year</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) of the focal functional group X</t>
-    </r>
-  </si>
-  <si>
     <t>mortality.fishing.recruitment.size.spX</t>
   </si>
   <si>
@@ -312,9 +288,6 @@
   </si>
   <si>
     <t>population.seeding.biomass.spX</t>
-  </si>
-  <si>
-    <t>Initial biomass (i.e., biomass in time step 0, in tons) of focal functional group X in the OSMOSE model</t>
   </si>
   <si>
     <t>plankton.name.plkX</t>
@@ -481,22 +454,10 @@
     <t>Name of the file containing estimates of fishing seasonality for functional group X</t>
   </si>
   <si>
-    <t>The user should enter a value for this parameter. The default value provided (25.24°N) is the value of the parameter in the OSMOSE model of the West Florida Shelf</t>
-  </si>
-  <si>
-    <t>The user should enter a value for this parameter. The default value provided (-80.16°E) is the value of the parameter in the OSMOSE model of the West Florida Shelf</t>
-  </si>
-  <si>
     <t>The user should enter a value for this parameter. The default value provided (39) is the value of the parameter in the OSMOSE model of the West Florida Shelf</t>
   </si>
   <si>
     <t>The user should enter a value for this parameter. The default value provided (33) is the value of the parameter in the OSMOSE model of the West Florida Shelf</t>
-  </si>
-  <si>
-    <t>The user should enter a value for this parameter. The default value provided (31.00°N) is the value of the parameter in the OSMOSE model of the West Florida Shelf</t>
-  </si>
-  <si>
-    <t>The user should enter a value for this parameter. The default value provided (-87.00°E) is the value of the parameter in the OSMOSE model of the West Florida Shelf</t>
   </si>
   <si>
     <t>The user should enter a value for this parameter. The default value provided is: 0.0 ton</t>
@@ -900,9 +861,6 @@
     <t>The name of the .csv file is: predation-accessibility.csv</t>
   </si>
   <si>
-    <t>The value of this parameter is: size. The user should not alter the value of this parameter</t>
-  </si>
-  <si>
     <t>Ages (in years) or body sizes (in cm) delineating the different age classes or the different size classes of focal functional group X for which diet compositions should be computed</t>
   </si>
   <si>
@@ -985,9 +943,6 @@
     </r>
   </si>
   <si>
-    <t># This file provides estimates of accessibility coefficients for age classes of focal functional groups and estimates of theoretical accessibitlity coefficients for background functional groups</t>
-  </si>
-  <si>
     <t># The "predation-accessibility.csv" file was generated by the bridge between FishBase/SeaLifeBase and OSMOSE</t>
   </si>
   <si>
@@ -1086,9 +1041,6 @@
     <t>Maximum size (size at infinity, in cm) of focal functional group X</t>
   </si>
   <si>
-    <t>Female:male sex ratio of focal functional group X</t>
-  </si>
-  <si>
     <r>
       <t>Annual number of eggs per gram of mature female (in eggs.g</t>
     </r>
@@ -1202,15 +1154,6 @@
     </r>
   </si>
   <si>
-    <t>The default value of this parameter is: 3.5 year-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The default value of this parameter is: 3.5 </t>
-  </si>
-  <si>
-    <t>The default value of this parameter is: 30</t>
-  </si>
-  <si>
     <t>This parameter is actually the body size at sexual maturity of focal functional group X. A default value of 0.0 cm is provided by the bridge between FishBase/SeaLifeBase and OSMOSE if it was unable to assign a value to this parameter from the information compiled in FishBase and SeaLifeBase</t>
   </si>
   <si>
@@ -1248,12 +1191,87 @@
   </si>
   <si>
     <t>Range (in years) of the age classes of focal functional groups for which OSMOSE computes outputs</t>
+  </si>
+  <si>
+    <t>Name of .csv file providing basic parameter estimates (e.g., parameters of the von Bertafanffy growth relationship) for focal functional groups</t>
+  </si>
+  <si>
+    <t>Proportion of females for focal functional group X</t>
+  </si>
+  <si>
+    <t>The user should enter a value for this parameter. The default value provided (25.24°N) is the value of the parameter for the OSMOSE model of the West Florida Shelf</t>
+  </si>
+  <si>
+    <t>The user should enter a value for this parameter. The default value provided (-80.16°E) is the value of the parameter for the OSMOSE model of the West Florida Shelf</t>
+  </si>
+  <si>
+    <t>The user should enter a value for this parameter. The default value provided (31.00°N) is the value of the parameter for the OSMOSE model of the West Florida Shelf</t>
+  </si>
+  <si>
+    <t>The user should enter a value for this parameter. The default value provided (-87.00°E) is the value of the parameter for the OSMOSE model of the West Florida Shelf</t>
+  </si>
+  <si>
+    <r>
+      <t>Annual fishing mortality rate (in year</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) of focal functional group X</t>
+    </r>
+  </si>
+  <si>
+    <t>Initial biomass (i.e., biomass at time step 0, in tons) of focal functional group X in the OSMOSE model</t>
+  </si>
+  <si>
+    <r>
+      <t>The default value of this parameter is: 3.5 year</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <t># This file provides estimates of accessibility coefficients for age classes of focal functional groups (determining the accessiblity of the age classes of focal functional groups to one another) and estimates of theoretical accessibility coefficients for background functional groups (describing the accessibility of bakcground focal functional groups to the age classes of focal functional groups)</t>
+  </si>
+  <si>
+    <t># Please note that the estimates provided here only account for the position of the predators in the water column relative to that of their potential prey. A coefficient of 0.8 means that there is strong overlap between the predator and its potential prey in the water column (e.g., because both the predator and its potential prey are benthic animals), a coefficient of 0.4 means that there is moderate overlap between the predator and its potential prey in the water column, and a coefficient of 0.08 means that there is little overlap between the predator and its potential prey in the water column. Thus, the user may want to alter some of the accessibility coefficients and theoretical accessibility coefficients provided by the bridge between FishBase/SeaLifeBase and OSMOSE; for example, a given predator may not be able to attack a given potential prey (e.g., because the potential prey has venomous spines), in which case the user may want to set the accessibility coefficient of the potential prey to the predator to 0</t>
+  </si>
+  <si>
+    <t>The default value of this parameter is: 3.5 3.5. Currently, the bridge between FishBase/SeaLifeBase and OSMOSE provides identical minimum predator/prey size ratio estimates for the juveniles and adults of focal functional group X. The user may want to alter these estimates to account for ontogenetic changes in diet patterns (e.g., to account for the fact that adults of focal functional group X have the ability to feed on prey that are twice smaller than them, while juveniles of focal functional group X are only able to feed on prey that are four times smaller than them)</t>
+  </si>
+  <si>
+    <t>The default value of this parameter is: 30 30. Currently, the bridge between FishBase/SeaLifeBase and OSMOSE provides identical maximum predator/prey size ratio estimates for the juveniles and adults of focal functional group X. The user may want to alter these estimates to account for ontogenetic changes in diet patterns (e.g., to account for the fact that, contrary to adults, juveniles of focal functional group X feed on very small organisms such as zooplankton)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1784,11 +1802,11 @@
     <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Commentaire" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1805,6 +1823,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1853,7 +1874,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1886,9 +1907,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1921,6 +1959,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2099,19 +2154,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.28515625" customWidth="1"/>
-    <col min="2" max="2" width="55.140625" customWidth="1"/>
+    <col min="1" max="1" width="40.33203125" customWidth="1"/>
+    <col min="2" max="2" width="55.109375" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="4" width="86.42578125" customWidth="1"/>
+    <col min="4" max="4" width="86.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2125,7 +2180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2139,7 +2194,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -2150,10 +2205,10 @@
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2167,7 +2222,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -2178,24 +2233,24 @@
         <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -2206,10 +2261,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -2220,10 +2275,10 @@
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -2237,7 +2292,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -2248,10 +2303,10 @@
         <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -2265,7 +2320,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -2279,7 +2334,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
@@ -2293,7 +2348,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
@@ -2307,12 +2362,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>6</v>
@@ -2321,7 +2376,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
@@ -2335,7 +2390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>35</v>
       </c>
@@ -2349,7 +2404,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
@@ -2363,7 +2418,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>39</v>
       </c>
@@ -2377,7 +2432,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>40</v>
       </c>
@@ -2391,12 +2446,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>62</v>
+        <v>327</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>6</v>
@@ -2405,7 +2460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>43</v>
       </c>
@@ -2419,7 +2474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>45</v>
       </c>
@@ -2433,7 +2488,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>47</v>
       </c>
@@ -2458,18 +2513,18 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="49.42578125" customWidth="1"/>
+    <col min="2" max="2" width="49.44140625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="103" customWidth="1"/>
+    <col min="4" max="4" width="85.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2483,60 +2538,60 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>151</v>
-      </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="32.25" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -2549,19 +2604,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
-    <col min="2" max="2" width="52.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="4" width="91.140625" customWidth="1"/>
+    <col min="2" max="2" width="52.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" customWidth="1"/>
+    <col min="4" max="4" width="80.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2575,134 +2630,133 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="32.25" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2714,15 +2768,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.85546875" customWidth="1"/>
-    <col min="2" max="2" width="51.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="82.7109375" customWidth="1"/>
+    <col min="1" max="1" width="48.88671875" customWidth="1"/>
+    <col min="2" max="2" width="51.88671875" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="82.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2736,12 +2790,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -2759,20 +2813,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="54" style="3" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="97.28515625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="3"/>
+    <col min="3" max="3" width="29.44140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="97.33203125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2786,18 +2840,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="32.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -2807,22 +2861,31 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="196.44140625" style="5" customWidth="1"/>
+    <col min="2" max="16384" width="11.5546875" style="5"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>279</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -2838,16 +2901,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -2859,16 +2922,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2886,19 +2951,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -2912,20 +2977,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="99.42578125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="46.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="42.88671875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="99.44140625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2939,704 +3004,704 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="B13" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="B15" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="3" t="s">
+    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B13" s="3" t="s">
+    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="B18" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="3" t="s">
+    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="3" t="s">
+    <row r="26" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="3" t="s">
+    <row r="29" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="3" t="s">
+    <row r="30" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="3" t="s">
+    <row r="31" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="3" t="s">
+    <row r="34" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="3" t="s">
+    <row r="37" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="B37" s="3" t="s">
+    <row r="49" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B41" s="3" t="s">
+      <c r="B50" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" s="3" t="s">
+      <c r="B51" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -3648,19 +3713,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="91.28515625" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="86.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3674,200 +3739,200 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>305</v>
+        <v>328</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3880,19 +3945,19 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="57.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="80.140625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="41.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="57.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="80.109375" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3906,88 +3971,88 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -3999,20 +4064,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="53.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="91.5703125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="42.88671875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="53.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="91.5546875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4026,116 +4091,116 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>139</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -4148,17 +4213,17 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -4176,14 +4241,14 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -4198,19 +4263,19 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45" style="5" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="98.7109375" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="5"/>
+    <col min="2" max="2" width="40.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="98.6640625" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4224,54 +4289,54 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="32.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="B5" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
@@ -4291,19 +4356,19 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="37.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="48.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="95" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="3"/>
+    <col min="5" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4317,18 +4382,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>86</v>
+        <v>334</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -4341,34 +4406,34 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="50.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="102" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="33.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="88.21875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -4382,102 +4447,102 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="3" t="s">
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B12" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>